<commit_message>
include coal phase out
</commit_message>
<xml_diff>
--- a/model/params.xlsx
+++ b/model/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/e11777102_student_tuwien_ac_at/Documents/Arbeit/git/IndustryTransPath/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{B426C2CA-3CF2-4FE3-B74F-86746B14DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92493DD4-F8DF-4BB8-8493-0490FFDAF979}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{B426C2CA-3CF2-4FE3-B74F-86746B14DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E6BC133-4DB5-4B3B-94F1-9FC264E0029C}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="2" xr2:uid="{EC234235-8C42-44A6-A799-E4D5FA147C26}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{EC234235-8C42-44A6-A799-E4D5FA147C26}"/>
   </bookViews>
   <sheets>
     <sheet name="SITE" sheetId="1" r:id="rId1"/>
@@ -1643,22 +1643,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.3046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15234375" style="3"/>
-    <col min="3" max="3" width="11.15234375" style="6"/>
-    <col min="5" max="5" width="11.3828125" style="3"/>
-    <col min="6" max="10" width="7.69140625" customWidth="1"/>
-    <col min="11" max="11" width="30.15234375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="84.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3"/>
+    <col min="3" max="3" width="11.140625" style="6"/>
+    <col min="5" max="5" width="11.42578125" style="3"/>
+    <col min="6" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="84.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>139</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>141</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>142</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>143</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>67</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>68</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>77</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>78</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>80</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>81</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>83</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>84</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>85</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>86</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>87</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>88</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>89</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>90</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>92</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>93</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>94</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>96</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>97</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>98</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>119</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>121</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>123</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>125</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>126</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>127</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>128</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>129</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>130</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>131</v>
       </c>
@@ -3249,9 +3249,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -3310,9 +3310,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -3370,9 +3370,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -3430,9 +3430,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -3490,9 +3490,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -3546,27 +3546,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B5898A-008C-4E7B-A92F-3F70998D2C26}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E44" sqref="E44"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.84375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.3046875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.69140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3828125" style="3"/>
-    <col min="7" max="7" width="7.3828125" style="3" customWidth="1"/>
-    <col min="8" max="12" width="7.53515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="37.84375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="105.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="3"/>
+    <col min="7" max="7" width="7.42578125" style="3" customWidth="1"/>
+    <col min="8" max="12" width="7.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="37.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="105.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>161</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>160</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>159</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>158</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>167</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>157</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>156</v>
       </c>
@@ -3940,10 +3940,10 @@
         <v>-0.25</v>
       </c>
       <c r="I11" s="3">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="J11" s="3">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="K11" s="3">
         <v>0</v>
@@ -3958,7 +3958,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>155</v>
       </c>
@@ -3984,10 +3984,10 @@
         <v>-0.25</v>
       </c>
       <c r="I12" s="3">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="J12" s="3">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="K12" s="3">
         <v>0</v>
@@ -4002,7 +4002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>154</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>153</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>152</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>151</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>164</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>150</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>149</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>148</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>147</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>146</v>
       </c>
@@ -4364,13 +4364,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6082AF7-273D-43BB-BA32-883A02C6370B}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>161</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>160</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>159</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>158</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>167</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>157</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>156</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>155</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>154</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>153</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>152</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>151</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>164</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>150</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>149</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>148</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>147</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>146</v>
       </c>
@@ -4576,9 +4576,9 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>161</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>160</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>159</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>158</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>167</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>157</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>156</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>155</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>154</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>153</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>152</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>151</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>164</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>150</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>149</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>148</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>147</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>146</v>
       </c>
@@ -4784,9 +4784,9 @@
       <selection activeCell="N38" sqref="N38:O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4795,7 +4795,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2024</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2027</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2029</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2031</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2032</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2033</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2034</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2035</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2036</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2037</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2038</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2039</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2040</v>
       </c>
@@ -4983,9 +4983,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5069,9 +5069,9 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5155,9 +5155,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5241,9 +5241,9 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>

</xml_diff>